<commit_message>
Updated Excel data file
</commit_message>
<xml_diff>
--- a/הכנסות והוצאות אבא ממאי ועד היום.xlsx
+++ b/הכנסות והוצאות אבא ממאי ועד היום.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myproject\anilses_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D014121-A772-4F91-A7AF-0424CFD4BF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF07992-0739-4B83-88A3-C5C8D844DDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="133">
   <si>
     <t>תאריך</t>
   </si>
@@ -323,6 +323,117 @@
   </si>
   <si>
     <t>בגדים גרבים ואוכל</t>
+  </si>
+  <si>
+    <t>לטובת: בני ועמית מימון עבור: תשלום מעיל</t>
+  </si>
+  <si>
+    <t>תשלום מעיל</t>
+  </si>
+  <si>
+    <t>לטובת: SACHIN CHANDRAPPA עבור: salary payment</t>
+  </si>
+  <si>
+    <t>salary payment</t>
+  </si>
+  <si>
+    <t>ני"ע-קניה</t>
+  </si>
+  <si>
+    <t>לטובת: אריאלה ועופר מימון עבור: קייטרינג 2 ,סופר,,קומקום</t>
+  </si>
+  <si>
+    <t>קייטרינג 2 ,סופר,,קומקום</t>
+  </si>
+  <si>
+    <t>החזרת שיק (תאריך ערך: 05/03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> סיבת החזרה:  שגיאה בהקלדת פרטי חשבון המושך או ב</t>
+  </si>
+  <si>
+    <t>סיבת החזרה:</t>
+  </si>
+  <si>
+    <t>שגיאה בהקלדת פרטי חשבון המושך או ב</t>
+  </si>
+  <si>
+    <t>הפקדת שיק חוזר</t>
+  </si>
+  <si>
+    <t>לטובת: SACHIN CHANDRAPPA עבור: salary of February 2025</t>
+  </si>
+  <si>
+    <t>salary of February 2025</t>
+  </si>
+  <si>
+    <t>לטובת: סוצקבר אלכסנדר עבור: תשלום גריאטר בדיקה אמא</t>
+  </si>
+  <si>
+    <t>סוצקבר אלכסנדר</t>
+  </si>
+  <si>
+    <t>תשלום גריאטר בדיקה אמא</t>
+  </si>
+  <si>
+    <t>לטובת: שרית ושמעון אטרף עבור: העברה של ביטחונות לבת שלי</t>
+  </si>
+  <si>
+    <t>העברה של ביטחונות לבת שלי</t>
+  </si>
+  <si>
+    <t>לטובת: אריאלה ועופר מימון עבור: העברה של ביטחונות בן עופר</t>
+  </si>
+  <si>
+    <t>העברה של ביטחונות בן עופר</t>
+  </si>
+  <si>
+    <t>לטובת: בני ועמית מימון עבור: אמא  לתשלום שכירות</t>
+  </si>
+  <si>
+    <t>אמא  לתשלום שכירות</t>
+  </si>
+  <si>
+    <t>לטובת: אנשים תמיד עבור: הרשמה ודמי תאגיד 3 חודשי</t>
+  </si>
+  <si>
+    <t>הרשמה ודמי תאגיד 3 חודשי</t>
+  </si>
+  <si>
+    <t>לטובת: SACHIN CHANDRAPPA עבור: salary March</t>
+  </si>
+  <si>
+    <t>salary March</t>
+  </si>
+  <si>
+    <t>העברה לבנק אחר</t>
+  </si>
+  <si>
+    <t>לטובת: בורקין מצבה בע"מ עבור: מצבה לאבא</t>
+  </si>
+  <si>
+    <t>בורקין מצבה בע"מ</t>
+  </si>
+  <si>
+    <t>מצבה לאבא</t>
+  </si>
+  <si>
+    <t>לטובת: אסתר ביטון עבור: קייטרינג לאזכרה חודש</t>
+  </si>
+  <si>
+    <t>אסתר ביטון</t>
+  </si>
+  <si>
+    <t>קייטרינג לאזכרה חודש</t>
+  </si>
+  <si>
+    <t>מסטרקרד</t>
+  </si>
+  <si>
+    <t>לטובת: SACHIN CHANDRAPPA עבור: salary 5 and obligations</t>
+  </si>
+  <si>
+    <t>salary 5 and obligations</t>
   </si>
 </sst>
 </file>
@@ -687,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:J217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4656,6 +4767,1752 @@
       </c>
       <c r="J151" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A152" s="2">
+        <v>45697</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D152" s="4">
+        <v>379647098</v>
+      </c>
+      <c r="E152" s="5">
+        <v>249</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G152" s="5">
+        <v>302591.99</v>
+      </c>
+      <c r="H152" s="2">
+        <v>45697</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A153" s="2">
+        <v>45697</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D153" s="4">
+        <v>379645735</v>
+      </c>
+      <c r="E153" s="5">
+        <v>3738</v>
+      </c>
+      <c r="F153" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G153" s="5">
+        <v>302840.99</v>
+      </c>
+      <c r="H153" s="2">
+        <v>45697</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A154" s="2">
+        <v>45698</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D154" s="4">
+        <v>706994</v>
+      </c>
+      <c r="E154" s="5">
+        <v>534.34</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" s="5">
+        <v>302057.65000000002</v>
+      </c>
+      <c r="H154" s="2">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A155" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D155" s="4">
+        <v>5136874</v>
+      </c>
+      <c r="E155" s="5">
+        <v>272049.93</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G155" s="5">
+        <v>30007.72</v>
+      </c>
+      <c r="H155" s="2">
+        <v>45699</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A156" s="2">
+        <v>45702</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D156" s="4">
+        <v>63051080</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" s="5">
+        <v>2528</v>
+      </c>
+      <c r="G156" s="5">
+        <v>32535.72</v>
+      </c>
+      <c r="H156" s="2">
+        <v>45702</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A157" s="2">
+        <v>45704</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D157" s="4">
+        <v>32349623</v>
+      </c>
+      <c r="E157" s="5">
+        <v>25</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="5">
+        <v>31410.720000000001</v>
+      </c>
+      <c r="H157" s="2">
+        <v>45704</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A158" s="2">
+        <v>45704</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D158" s="4">
+        <v>2590001</v>
+      </c>
+      <c r="E158" s="5">
+        <v>1100</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" s="5">
+        <v>31435.72</v>
+      </c>
+      <c r="H158" s="2">
+        <v>45704</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A159" s="2">
+        <v>45708</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D159" s="4">
+        <v>703991</v>
+      </c>
+      <c r="E159" s="5">
+        <v>48.93</v>
+      </c>
+      <c r="F159" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" s="5">
+        <v>31361.79</v>
+      </c>
+      <c r="H159" s="2">
+        <v>45708</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A160" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D160" s="4">
+        <v>60697083</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F160" s="5">
+        <v>2287</v>
+      </c>
+      <c r="G160" s="5">
+        <v>47653.67</v>
+      </c>
+      <c r="H160" s="2">
+        <v>45716</v>
+      </c>
+      <c r="J160" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A161" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D161" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F161" s="5">
+        <v>2616</v>
+      </c>
+      <c r="G161" s="5">
+        <v>45366.67</v>
+      </c>
+      <c r="H161" s="2">
+        <v>45716</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A162" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F162" s="5">
+        <v>3801</v>
+      </c>
+      <c r="G162" s="5">
+        <v>42750.67</v>
+      </c>
+      <c r="H162" s="2">
+        <v>45716</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A163" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D163" s="4">
+        <v>4061016</v>
+      </c>
+      <c r="E163" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F163" s="5">
+        <v>7587.88</v>
+      </c>
+      <c r="G163" s="5">
+        <v>38949.67</v>
+      </c>
+      <c r="H163" s="2">
+        <v>45716</v>
+      </c>
+      <c r="J163" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A164" s="2">
+        <v>45718</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D164" s="4">
+        <v>7302256</v>
+      </c>
+      <c r="E164" s="5">
+        <v>5300</v>
+      </c>
+      <c r="F164" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G164" s="5">
+        <v>37259.1</v>
+      </c>
+      <c r="H164" s="2">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A165" s="2">
+        <v>45718</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D165" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E165" s="5">
+        <v>4093.57</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G165" s="5">
+        <v>42559.1</v>
+      </c>
+      <c r="H165" s="2">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A166" s="2">
+        <v>45718</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D166" s="4">
+        <v>383156972</v>
+      </c>
+      <c r="E166" s="5">
+        <v>1001</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G166" s="5">
+        <v>46652.67</v>
+      </c>
+      <c r="H166" s="2">
+        <v>45718</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J166" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A167" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="4">
+        <v>7</v>
+      </c>
+      <c r="E167" s="5">
+        <v>12.25</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G167" s="5">
+        <v>37236.85</v>
+      </c>
+      <c r="H167" s="2">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A168" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D168" s="4">
+        <v>817</v>
+      </c>
+      <c r="E168" s="5">
+        <v>10</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G168" s="5">
+        <v>37249.1</v>
+      </c>
+      <c r="H168" s="2">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A169" s="2">
+        <v>45721</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D169" s="4">
+        <v>20000098</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F169" s="5">
+        <v>3200</v>
+      </c>
+      <c r="G169" s="5">
+        <v>40436.85</v>
+      </c>
+      <c r="H169" s="2">
+        <v>45721</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A170" s="2">
+        <v>45722</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D170" s="4">
+        <v>20000098</v>
+      </c>
+      <c r="E170" s="5">
+        <v>3200</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G170" s="5">
+        <v>37236.85</v>
+      </c>
+      <c r="H170" s="2">
+        <v>45721</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J170" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A171" s="2">
+        <v>45723</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D171" s="4">
+        <v>286010777</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F171" s="5">
+        <v>3200</v>
+      </c>
+      <c r="G171" s="5">
+        <v>40436.85</v>
+      </c>
+      <c r="H171" s="2">
+        <v>45723</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A172" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D172" s="4">
+        <v>384726192</v>
+      </c>
+      <c r="E172" s="5">
+        <v>4064</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G172" s="5">
+        <v>36372.85</v>
+      </c>
+      <c r="H172" s="2">
+        <v>45726</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A173" s="2">
+        <v>45732</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D173" s="4">
+        <v>32349623</v>
+      </c>
+      <c r="E173" s="5">
+        <v>25</v>
+      </c>
+      <c r="F173" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G173" s="5">
+        <v>35247.85</v>
+      </c>
+      <c r="H173" s="2">
+        <v>45732</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A174" s="2">
+        <v>45732</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D174" s="4">
+        <v>2590001</v>
+      </c>
+      <c r="E174" s="5">
+        <v>1100</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G174" s="5">
+        <v>35272.85</v>
+      </c>
+      <c r="H174" s="2">
+        <v>45732</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A175" s="2">
+        <v>45735</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D175" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E175" s="5">
+        <v>1500</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G175" s="5">
+        <v>33747.85</v>
+      </c>
+      <c r="H175" s="2">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A176" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D176" s="4">
+        <v>387144806</v>
+      </c>
+      <c r="E176" s="5">
+        <v>1800</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176" s="5">
+        <v>30651.85</v>
+      </c>
+      <c r="H176" s="2">
+        <v>45740</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J176" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A177" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D177" s="4">
+        <v>387081799</v>
+      </c>
+      <c r="E177" s="5">
+        <v>10000</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G177" s="5">
+        <v>32451.85</v>
+      </c>
+      <c r="H177" s="2">
+        <v>45740</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J177" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A178" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D178" s="4">
+        <v>60697083</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F178" s="5">
+        <v>2287</v>
+      </c>
+      <c r="G178" s="5">
+        <v>42451.85</v>
+      </c>
+      <c r="H178" s="2">
+        <v>45740</v>
+      </c>
+      <c r="J178" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A179" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D179" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F179" s="5">
+        <v>2616</v>
+      </c>
+      <c r="G179" s="5">
+        <v>40164.85</v>
+      </c>
+      <c r="H179" s="2">
+        <v>45740</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A180" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D180" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F180" s="5">
+        <v>3801</v>
+      </c>
+      <c r="G180" s="5">
+        <v>37548.85</v>
+      </c>
+      <c r="H180" s="2">
+        <v>45740</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A181" s="2">
+        <v>45741</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D181" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E181" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G181" s="5">
+        <v>5651.85</v>
+      </c>
+      <c r="H181" s="2">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A182" s="2">
+        <v>45741</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D182" s="4">
+        <v>387275982</v>
+      </c>
+      <c r="E182" s="5">
+        <v>20000</v>
+      </c>
+      <c r="F182" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G182" s="5">
+        <v>10651.85</v>
+      </c>
+      <c r="H182" s="2">
+        <v>45741</v>
+      </c>
+      <c r="I182" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J182" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A183" s="2">
+        <v>45743</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D183" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E183" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F183" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G183" s="5">
+        <v>51931.35</v>
+      </c>
+      <c r="H183" s="2">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A184" s="2">
+        <v>45743</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D184" s="4">
+        <v>850001</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F184" s="5">
+        <v>1279.5</v>
+      </c>
+      <c r="G184" s="5">
+        <v>56931.35</v>
+      </c>
+      <c r="H184" s="2">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A185" s="2">
+        <v>45743</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D185" s="4">
+        <v>850001</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F185" s="5">
+        <v>50000</v>
+      </c>
+      <c r="G185" s="5">
+        <v>55651.85</v>
+      </c>
+      <c r="H185" s="2">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A186" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D186" s="4">
+        <v>388080722</v>
+      </c>
+      <c r="E186" s="5">
+        <v>5300</v>
+      </c>
+      <c r="F186" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186" s="5">
+        <v>54219.23</v>
+      </c>
+      <c r="H186" s="2">
+        <v>45747</v>
+      </c>
+      <c r="I186" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J186" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A187" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187" s="4">
+        <v>4061016</v>
+      </c>
+      <c r="E187" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F187" s="5">
+        <v>7587.88</v>
+      </c>
+      <c r="G187" s="5">
+        <v>59519.23</v>
+      </c>
+      <c r="H187" s="2">
+        <v>45747</v>
+      </c>
+      <c r="J187" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A188" s="2">
+        <v>45748</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D188" s="4">
+        <v>7302257</v>
+      </c>
+      <c r="E188" s="5">
+        <v>5300</v>
+      </c>
+      <c r="F188" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G188" s="5">
+        <v>48919.23</v>
+      </c>
+      <c r="H188" s="2">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A189" s="2">
+        <v>45749</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D189" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E189" s="5">
+        <v>6955.73</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G189" s="5">
+        <v>41413.5</v>
+      </c>
+      <c r="H189" s="2">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A190" s="2">
+        <v>45749</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D190" s="4">
+        <v>388639038</v>
+      </c>
+      <c r="E190" s="5">
+        <v>1010</v>
+      </c>
+      <c r="F190" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G190" s="5">
+        <v>48369.23</v>
+      </c>
+      <c r="H190" s="2">
+        <v>45749</v>
+      </c>
+      <c r="I190" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J190" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A191" s="2">
+        <v>45749</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D191" s="4">
+        <v>86405206</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F191" s="5">
+        <v>460</v>
+      </c>
+      <c r="G191" s="5">
+        <v>49379.23</v>
+      </c>
+      <c r="H191" s="2">
+        <v>45749</v>
+      </c>
+      <c r="J191" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A192" s="2">
+        <v>45750</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D192" s="4">
+        <v>7</v>
+      </c>
+      <c r="E192" s="5">
+        <v>12.25</v>
+      </c>
+      <c r="F192" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G192" s="5">
+        <v>41617.040000000001</v>
+      </c>
+      <c r="H192" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A193" s="2">
+        <v>45750</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D193" s="4">
+        <v>817</v>
+      </c>
+      <c r="E193" s="5">
+        <v>10</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G193" s="5">
+        <v>41629.29</v>
+      </c>
+      <c r="H193" s="2">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A194" s="2">
+        <v>45750</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" s="4">
+        <v>80518327</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F194" s="5">
+        <v>225.79</v>
+      </c>
+      <c r="G194" s="5">
+        <v>41639.29</v>
+      </c>
+      <c r="H194" s="2">
+        <v>45750</v>
+      </c>
+      <c r="J194" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A195" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D195" s="4">
+        <v>80000099</v>
+      </c>
+      <c r="E195" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F195" s="5">
+        <v>3200</v>
+      </c>
+      <c r="G195" s="5">
+        <v>44817.04</v>
+      </c>
+      <c r="H195" s="2">
+        <v>45753</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A196" s="2">
+        <v>45757</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D196" s="4">
+        <v>706994</v>
+      </c>
+      <c r="E196" s="5">
+        <v>835.01</v>
+      </c>
+      <c r="F196" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G196" s="5">
+        <v>40440.03</v>
+      </c>
+      <c r="H196" s="2">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A197" s="2">
+        <v>45757</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D197" s="4">
+        <v>390263163</v>
+      </c>
+      <c r="E197" s="5">
+        <v>3542</v>
+      </c>
+      <c r="F197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G197" s="5">
+        <v>41275.040000000001</v>
+      </c>
+      <c r="H197" s="2">
+        <v>45757</v>
+      </c>
+      <c r="I197" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J197" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A198" s="2">
+        <v>45761</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D198" s="4">
+        <v>10409419</v>
+      </c>
+      <c r="E198" s="5">
+        <v>10500</v>
+      </c>
+      <c r="F198" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G198" s="5">
+        <v>41630.03</v>
+      </c>
+      <c r="H198" s="2">
+        <v>45761</v>
+      </c>
+      <c r="I198" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J198" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A199" s="2">
+        <v>45761</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D199" s="4">
+        <v>63051080</v>
+      </c>
+      <c r="E199" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F199" s="5">
+        <v>1422</v>
+      </c>
+      <c r="G199" s="5">
+        <v>52130.03</v>
+      </c>
+      <c r="H199" s="2">
+        <v>45761</v>
+      </c>
+      <c r="J199" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A200" s="2">
+        <v>45761</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D200" s="4">
+        <v>63051080</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F200" s="5">
+        <v>10268</v>
+      </c>
+      <c r="G200" s="5">
+        <v>50708.03</v>
+      </c>
+      <c r="H200" s="2">
+        <v>45761</v>
+      </c>
+      <c r="J200" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A201" s="2">
+        <v>45762</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D201" s="4">
+        <v>2590001</v>
+      </c>
+      <c r="E201" s="5">
+        <v>1100</v>
+      </c>
+      <c r="F201" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G201" s="5">
+        <v>40530.03</v>
+      </c>
+      <c r="H201" s="2">
+        <v>45762</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A202" s="2">
+        <v>45763</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D202" s="4">
+        <v>32349623</v>
+      </c>
+      <c r="E202" s="5">
+        <v>25</v>
+      </c>
+      <c r="F202" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G202" s="5">
+        <v>37805.03</v>
+      </c>
+      <c r="H202" s="2">
+        <v>45763</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A203" s="2">
+        <v>45763</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D203" s="4">
+        <v>391263302</v>
+      </c>
+      <c r="E203" s="5">
+        <v>2700</v>
+      </c>
+      <c r="F203" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G203" s="5">
+        <v>37830.03</v>
+      </c>
+      <c r="H203" s="2">
+        <v>45763</v>
+      </c>
+      <c r="I203" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A204" s="2">
+        <v>45767</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D204" s="4">
+        <v>703991</v>
+      </c>
+      <c r="E204" s="5">
+        <v>49.16</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G204" s="5">
+        <v>37755.870000000003</v>
+      </c>
+      <c r="H204" s="2">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A205" s="2">
+        <v>45770</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D205" s="4">
+        <v>60697083</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F205" s="5">
+        <v>2413</v>
+      </c>
+      <c r="G205" s="5">
+        <v>42553.87</v>
+      </c>
+      <c r="H205" s="2">
+        <v>45770</v>
+      </c>
+      <c r="J205" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A206" s="2">
+        <v>45770</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D206" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F206" s="5">
+        <v>2385</v>
+      </c>
+      <c r="G206" s="5">
+        <v>40140.870000000003</v>
+      </c>
+      <c r="H206" s="2">
+        <v>45770</v>
+      </c>
+      <c r="J206" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A207" s="2">
+        <v>45779</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D207" s="4">
+        <v>7302265</v>
+      </c>
+      <c r="E207" s="5">
+        <v>5300</v>
+      </c>
+      <c r="F207" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" s="5">
+        <v>36791.18</v>
+      </c>
+      <c r="H207" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A208" s="2">
+        <v>45779</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D208" s="4">
+        <v>961</v>
+      </c>
+      <c r="E208" s="5">
+        <v>267.38</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" s="5">
+        <v>42091.18</v>
+      </c>
+      <c r="H208" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A209" s="2">
+        <v>45779</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D209" s="4">
+        <v>9234</v>
+      </c>
+      <c r="E209" s="5">
+        <v>195.31</v>
+      </c>
+      <c r="F209" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G209" s="5">
+        <v>42358.559999999998</v>
+      </c>
+      <c r="H209" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A210" s="2">
+        <v>45781</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D210" s="4">
+        <v>5</v>
+      </c>
+      <c r="E210" s="5">
+        <v>8.75</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G210" s="5">
+        <v>39972.43</v>
+      </c>
+      <c r="H210" s="2">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A211" s="2">
+        <v>45781</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D211" s="4">
+        <v>817</v>
+      </c>
+      <c r="E211" s="5">
+        <v>10</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G211" s="5">
+        <v>39981.18</v>
+      </c>
+      <c r="H211" s="2">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A212" s="2">
+        <v>45781</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D212" s="4">
+        <v>80000100</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F212" s="5">
+        <v>3200</v>
+      </c>
+      <c r="G212" s="5">
+        <v>39991.18</v>
+      </c>
+      <c r="H212" s="2">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A213" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D213" s="4">
+        <v>395100508</v>
+      </c>
+      <c r="E213" s="5">
+        <v>8519</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G213" s="5">
+        <v>31453.43</v>
+      </c>
+      <c r="H213" s="2">
+        <v>45788</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J213" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A214" s="2">
+        <v>45792</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D214" s="4">
+        <v>2590001</v>
+      </c>
+      <c r="E214" s="5">
+        <v>1100</v>
+      </c>
+      <c r="F214" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G214" s="5">
+        <v>30353.43</v>
+      </c>
+      <c r="H214" s="2">
+        <v>45792</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A215" s="2">
+        <v>45795</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D215" s="4">
+        <v>32349623</v>
+      </c>
+      <c r="E215" s="5">
+        <v>25</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G215" s="5">
+        <v>30328.43</v>
+      </c>
+      <c r="H215" s="2">
+        <v>45795</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A216" s="2">
+        <v>45805</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D216" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E216" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F216" s="5">
+        <v>1422</v>
+      </c>
+      <c r="G216" s="5">
+        <v>34135.43</v>
+      </c>
+      <c r="H216" s="2">
+        <v>45805</v>
+      </c>
+      <c r="J216" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A217" s="2">
+        <v>45805</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D217" s="4">
+        <v>13101084</v>
+      </c>
+      <c r="E217" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F217" s="5">
+        <v>2385</v>
+      </c>
+      <c r="G217" s="5">
+        <v>32713.43</v>
+      </c>
+      <c r="H217" s="2">
+        <v>45805</v>
+      </c>
+      <c r="J217" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>